<commit_message>
Added chatbot feature, updated README, added result screenshots
</commit_message>
<xml_diff>
--- a/invoice_analysis_export.xlsx
+++ b/invoice_analysis_export.xlsx
@@ -469,7 +469,7 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>Status: Declined
-Reason: The invoice does not meet the policy guidelines for reimbursement of food expenses. The policy specifies a limit of ₹200 per meal, whereas the total amount on the invoice is ₹88.00, which is also not clearly broken down into individual meals. Additionally, the receipt is from a restaurant in Los Angeles, USA, whereas the company policy is for IAI Solution, an Indian company, and the policy specifies rupee amounts.</t>
+Reason: The invoice is for food and beverages, but the total amount is ₹88.00, which exceeds the allowed limit of ₹200 per the policy. Additionally, there is no indication that the meal was incurred while traveling for work or attending business meetings, which is a requirement for reimbursement.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -497,7 +497,7 @@
       <c r="C3" t="inlineStr">
         <is>
           <t>Status: Declined
-Reason: The invoice contains an item "Royal Stag Whisky" which is an alcoholic beverage, and as per the policy (Section 5.1, Restrictions), alcoholic beverages are not reimbursable.</t>
+Reason: The invoice includes Alcoholic beverages (Royal Stag Whisky) which are not reimbursable as per the policy (Section 5.1 Restrictions).</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -525,7 +525,7 @@
       <c r="C4" t="inlineStr">
         <is>
           <t>Status: Declined
-Reason: The invoice is for Wines, which is an alcoholic beverage, and is therefore not reimbursable as per the policy (Section 5.1 Restrictions).</t>
+Reason: The invoice includes reimbursement for wines, which are explicitly restricted under the Food and Beverages category in the policy. Additionally, the total amount of ₹ 1100.4 exceeds the food allowance of ₹200 per meal set by the policy.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">

</xml_diff>